<commit_message>
SE-2931: Update Data File
</commit_message>
<xml_diff>
--- a/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
+++ b/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\GitHub\sample-notebooks\examples\use-cases\abor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D206748A-3148-453D-8528-3F09008D02D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F176B0E-7610-42F8-87E7-044B8D695253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="87">
   <si>
     <t>Asset</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>account/coa-testing/FundManagerName</t>
   </si>
   <si>
     <t>LocalCountryReference</t>
@@ -655,7 +652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -669,14 +666,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -690,27 +687,27 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -724,7 +721,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -738,7 +735,7 @@
         <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -755,14 +752,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -776,7 +773,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -784,13 +781,13 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -798,13 +795,13 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -812,10 +809,10 @@
         <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -829,15 +826,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -860,10 +857,10 @@
         <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -886,7 +883,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -909,7 +906,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -932,7 +929,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -955,7 +952,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -978,7 +975,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1024,7 +1021,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1047,7 +1044,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1070,7 +1067,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1093,7 +1090,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1116,7 +1113,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1139,7 +1136,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1162,7 +1159,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1185,7 +1182,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1208,7 +1205,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1231,7 +1228,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1254,7 +1251,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1277,7 +1274,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1300,7 +1297,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1323,7 +1320,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1346,7 +1343,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1369,7 +1366,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1415,7 +1412,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1438,7 +1435,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1461,7 +1458,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1484,7 +1481,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1504,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1553,7 +1550,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1576,7 +1573,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1599,7 +1596,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1622,10 +1619,10 @@
         <v>68</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1648,7 +1645,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1671,7 +1668,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1694,7 +1691,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1717,7 +1714,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1763,7 +1760,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1786,7 +1783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1809,7 +1806,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1832,7 +1829,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1855,7 +1852,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1878,7 +1875,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1901,7 +1898,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1924,7 +1921,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1947,7 +1944,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1970,7 +1967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1993,7 +1990,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2016,7 +2013,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2039,7 +2036,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -2062,7 +2059,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2085,10 +2082,10 @@
         <v>69</v>
       </c>
       <c r="H54" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -2111,7 +2108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -2134,7 +2131,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -2157,7 +2154,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -2180,7 +2177,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -2203,7 +2200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -2226,7 +2223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -2249,7 +2246,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2272,7 +2269,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>42</v>
       </c>
@@ -2295,7 +2292,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -2318,7 +2315,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -2341,7 +2338,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -2364,7 +2361,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>42</v>
       </c>
@@ -2387,7 +2384,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>42</v>
       </c>
@@ -2410,7 +2407,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>42</v>
       </c>
@@ -2433,7 +2430,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -2456,7 +2453,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -2479,7 +2476,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -2502,7 +2499,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -2525,7 +2522,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -2548,7 +2545,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -2571,7 +2568,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -2594,7 +2591,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -2617,7 +2614,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -2640,10 +2637,10 @@
         <v>68</v>
       </c>
       <c r="H78" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -2666,7 +2663,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -2689,7 +2686,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -2712,7 +2709,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>42</v>
       </c>
@@ -2735,7 +2732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -2758,7 +2755,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -2781,7 +2778,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -2804,7 +2801,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -2827,7 +2824,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>42</v>
       </c>
@@ -2850,7 +2847,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>42</v>
       </c>
@@ -2873,7 +2870,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>42</v>
       </c>
@@ -2896,7 +2893,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>42</v>
       </c>
@@ -2919,7 +2916,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -2942,7 +2939,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>42</v>
       </c>
@@ -2965,7 +2962,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>42</v>
       </c>
@@ -2988,7 +2985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>42</v>
       </c>
@@ -3011,7 +3008,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>42</v>
       </c>
@@ -3034,7 +3031,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>42</v>
       </c>
@@ -3057,7 +3054,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>42</v>
       </c>
@@ -3080,7 +3077,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>42</v>
       </c>
@@ -3103,7 +3100,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>42</v>
       </c>
@@ -3126,7 +3123,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>42</v>
       </c>
@@ -3149,7 +3146,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -3172,7 +3169,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>42</v>
       </c>
@@ -3195,7 +3192,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>42</v>
       </c>
@@ -3218,7 +3215,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>42</v>
       </c>
@@ -3241,7 +3238,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>42</v>
       </c>
@@ -3264,7 +3261,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>42</v>
       </c>
@@ -3287,7 +3284,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>42</v>
       </c>
@@ -3310,10 +3307,10 @@
         <v>69</v>
       </c>
       <c r="H107" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>42</v>
       </c>
@@ -3336,7 +3333,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>42</v>
       </c>
@@ -3359,7 +3356,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>42</v>
       </c>
@@ -3382,7 +3379,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>42</v>
       </c>
@@ -3405,7 +3402,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>42</v>
       </c>
@@ -3428,7 +3425,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>42</v>
       </c>
@@ -3451,7 +3448,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>42</v>
       </c>
@@ -3474,7 +3471,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>42</v>
       </c>
@@ -3497,7 +3494,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>42</v>
       </c>
@@ -3520,7 +3517,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>42</v>
       </c>
@@ -3543,7 +3540,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>42</v>
       </c>
@@ -3566,7 +3563,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>42</v>
       </c>
@@ -3589,7 +3586,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>42</v>
       </c>
@@ -3612,7 +3609,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>42</v>
       </c>
@@ -3635,7 +3632,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -3658,7 +3655,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>42</v>
       </c>
@@ -3681,7 +3678,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>42</v>
       </c>
@@ -3704,7 +3701,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>42</v>
       </c>
@@ -3727,7 +3724,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>42</v>
       </c>
@@ -3750,7 +3747,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>42</v>
       </c>
@@ -3773,7 +3770,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>42</v>
       </c>
@@ -3796,7 +3793,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>42</v>
       </c>
@@ -3819,7 +3816,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>42</v>
       </c>
@@ -3842,7 +3839,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>42</v>
       </c>
@@ -3865,7 +3862,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>42</v>
       </c>
@@ -3888,7 +3885,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>42</v>
       </c>
@@ -3911,7 +3908,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>42</v>
       </c>
@@ -3934,7 +3931,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>42</v>
       </c>
@@ -3957,7 +3954,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>42</v>
       </c>
@@ -3980,7 +3977,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>42</v>
       </c>
@@ -4003,7 +4000,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>42</v>
       </c>
@@ -4026,7 +4023,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>42</v>
       </c>
@@ -4049,7 +4046,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -4072,7 +4069,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>42</v>
       </c>
@@ -4095,7 +4092,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>42</v>
       </c>
@@ -4118,7 +4115,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>42</v>
       </c>
@@ -4141,7 +4138,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>42</v>
       </c>
@@ -4164,7 +4161,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>42</v>
       </c>
@@ -4187,7 +4184,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>42</v>
       </c>
@@ -4210,7 +4207,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -4233,7 +4230,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>42</v>
       </c>
@@ -4256,7 +4253,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>42</v>
       </c>
@@ -4279,7 +4276,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>42</v>
       </c>
@@ -4302,7 +4299,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>42</v>
       </c>
@@ -4325,7 +4322,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>42</v>
       </c>
@@ -4348,7 +4345,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -4371,7 +4368,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>42</v>
       </c>
@@ -4394,7 +4391,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>42</v>
       </c>
@@ -4417,7 +4414,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>42</v>
       </c>
@@ -4440,7 +4437,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>42</v>
       </c>
@@ -4463,7 +4460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -4486,7 +4483,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -4509,7 +4506,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>42</v>
       </c>
@@ -4532,7 +4529,7 @@
         <v>69</v>
       </c>
       <c r="H160" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4546,17 +4543,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -4573,7 +4570,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -4584,13 +4581,13 @@
         <v>300000</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -4601,13 +4598,13 @@
         <v>770000</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -4618,13 +4615,13 @@
         <v>242200</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -4635,13 +4632,13 @@
         <v>770000</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -4652,10 +4649,10 @@
         <v>770000</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IBOR-568 update for tighter validation when adding properties
</commit_message>
<xml_diff>
--- a/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
+++ b/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\GitHub\sample-notebooks\examples\use-cases\abor\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rizwansaeed/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F176B0E-7610-42F8-87E7-044B8D695253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4AB24D-ADC6-E041-86AE-F4B2B74A401A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
+    <workbookView xWindow="18780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart Of Accounts" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="88">
   <si>
     <t>Asset</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Dividend Expense due to Short Updated</t>
+  </si>
+  <si>
+    <t>UK</t>
   </si>
 </sst>
 </file>
@@ -662,18 +665,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFADDA2E-8A45-4DD9-A512-DA66470628BF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -690,7 +693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -707,7 +710,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -720,8 +723,11 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -752,14 +758,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -773,7 +779,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -787,7 +793,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -801,7 +807,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -824,17 +830,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548BBB04-43B1-4007-A99D-E53D85A6EB52}">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A71" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -860,7 +866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -883,7 +889,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -906,7 +912,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -929,7 +935,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -952,7 +958,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -975,7 +981,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1205,7 +1211,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1297,7 +1303,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1573,7 +1579,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1596,7 +1602,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1806,7 +1812,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1898,7 +1904,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1967,7 +1973,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2065,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -2108,7 +2114,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -2131,7 +2137,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -2200,7 +2206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>42</v>
       </c>
@@ -2292,7 +2298,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>42</v>
       </c>
@@ -2384,7 +2390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>42</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>42</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -2476,7 +2482,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -2522,7 +2528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -2545,7 +2551,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -2568,7 +2574,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -2591,7 +2597,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -2640,7 +2646,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2692,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>42</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -2755,7 +2761,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -2778,7 +2784,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -2824,7 +2830,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>42</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>42</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>42</v>
       </c>
@@ -2893,7 +2899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>42</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -2939,7 +2945,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>42</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>42</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>42</v>
       </c>
@@ -3008,7 +3014,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>42</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>42</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>42</v>
       </c>
@@ -3077,7 +3083,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>42</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>42</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>42</v>
       </c>
@@ -3146,7 +3152,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>42</v>
       </c>
@@ -3192,7 +3198,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>42</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>42</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>42</v>
       </c>
@@ -3261,7 +3267,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>42</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>42</v>
       </c>
@@ -3310,7 +3316,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>42</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>42</v>
       </c>
@@ -3356,7 +3362,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>42</v>
       </c>
@@ -3379,7 +3385,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>42</v>
       </c>
@@ -3402,7 +3408,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>42</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>42</v>
       </c>
@@ -3448,7 +3454,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>42</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>42</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>42</v>
       </c>
@@ -3517,7 +3523,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>42</v>
       </c>
@@ -3540,7 +3546,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>42</v>
       </c>
@@ -3563,7 +3569,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>42</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>42</v>
       </c>
@@ -3609,7 +3615,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>42</v>
       </c>
@@ -3632,7 +3638,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>42</v>
       </c>
@@ -3678,7 +3684,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>42</v>
       </c>
@@ -3701,7 +3707,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>42</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>42</v>
       </c>
@@ -3747,7 +3753,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>42</v>
       </c>
@@ -3770,7 +3776,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>42</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>42</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>42</v>
       </c>
@@ -3839,7 +3845,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>42</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>42</v>
       </c>
@@ -3885,7 +3891,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>42</v>
       </c>
@@ -3908,7 +3914,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>42</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>42</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>42</v>
       </c>
@@ -3977,7 +3983,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>42</v>
       </c>
@@ -4000,7 +4006,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>42</v>
       </c>
@@ -4023,7 +4029,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>42</v>
       </c>
@@ -4046,7 +4052,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -4069,7 +4075,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>42</v>
       </c>
@@ -4092,7 +4098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>42</v>
       </c>
@@ -4115,7 +4121,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>42</v>
       </c>
@@ -4138,7 +4144,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>42</v>
       </c>
@@ -4161,7 +4167,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>42</v>
       </c>
@@ -4184,7 +4190,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>42</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -4230,7 +4236,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>42</v>
       </c>
@@ -4253,7 +4259,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>42</v>
       </c>
@@ -4276,7 +4282,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>42</v>
       </c>
@@ -4299,7 +4305,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>42</v>
       </c>
@@ -4322,7 +4328,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>42</v>
       </c>
@@ -4345,7 +4351,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -4368,7 +4374,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>42</v>
       </c>
@@ -4391,7 +4397,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>42</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>42</v>
       </c>
@@ -4437,7 +4443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>42</v>
       </c>
@@ -4460,7 +4466,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -4506,7 +4512,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>42</v>
       </c>
@@ -4542,18 +4548,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431E17FB-41C8-40BE-942D-5C20ADEE04C5}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -4570,7 +4576,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -4587,7 +4593,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -4604,7 +4610,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -4621,7 +4627,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -4638,7 +4644,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
IBOR-568 update for tighter validation when adding properties (#717)
</commit_message>
<xml_diff>
--- a/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
+++ b/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\GitHub\sample-notebooks\examples\use-cases\abor\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rizwansaeed/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F176B0E-7610-42F8-87E7-044B8D695253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4AB24D-ADC6-E041-86AE-F4B2B74A401A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
+    <workbookView xWindow="18780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart Of Accounts" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="88">
   <si>
     <t>Asset</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Dividend Expense due to Short Updated</t>
+  </si>
+  <si>
+    <t>UK</t>
   </si>
 </sst>
 </file>
@@ -662,18 +665,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFADDA2E-8A45-4DD9-A512-DA66470628BF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -690,7 +693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -707,7 +710,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -720,8 +723,11 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -752,14 +758,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -773,7 +779,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -787,7 +793,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -801,7 +807,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -824,17 +830,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548BBB04-43B1-4007-A99D-E53D85A6EB52}">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A71" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -860,7 +866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -883,7 +889,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -906,7 +912,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -929,7 +935,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -952,7 +958,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -975,7 +981,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1205,7 +1211,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1297,7 +1303,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1573,7 +1579,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1596,7 +1602,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1806,7 +1812,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1898,7 +1904,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1967,7 +1973,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2065,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -2108,7 +2114,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -2131,7 +2137,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -2200,7 +2206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>42</v>
       </c>
@@ -2292,7 +2298,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>42</v>
       </c>
@@ -2384,7 +2390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>42</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>42</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -2476,7 +2482,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -2522,7 +2528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -2545,7 +2551,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -2568,7 +2574,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -2591,7 +2597,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -2640,7 +2646,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2692,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>42</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -2755,7 +2761,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -2778,7 +2784,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -2824,7 +2830,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>42</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>42</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>42</v>
       </c>
@@ -2893,7 +2899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>42</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -2939,7 +2945,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>42</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>42</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>42</v>
       </c>
@@ -3008,7 +3014,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>42</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>42</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>42</v>
       </c>
@@ -3077,7 +3083,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>42</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>42</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>42</v>
       </c>
@@ -3146,7 +3152,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>42</v>
       </c>
@@ -3192,7 +3198,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>42</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>42</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>42</v>
       </c>
@@ -3261,7 +3267,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>42</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>42</v>
       </c>
@@ -3310,7 +3316,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>42</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>42</v>
       </c>
@@ -3356,7 +3362,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>42</v>
       </c>
@@ -3379,7 +3385,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>42</v>
       </c>
@@ -3402,7 +3408,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>42</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>42</v>
       </c>
@@ -3448,7 +3454,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>42</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>42</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>42</v>
       </c>
@@ -3517,7 +3523,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>42</v>
       </c>
@@ -3540,7 +3546,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>42</v>
       </c>
@@ -3563,7 +3569,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>42</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>42</v>
       </c>
@@ -3609,7 +3615,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>42</v>
       </c>
@@ -3632,7 +3638,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>42</v>
       </c>
@@ -3678,7 +3684,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>42</v>
       </c>
@@ -3701,7 +3707,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>42</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>42</v>
       </c>
@@ -3747,7 +3753,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>42</v>
       </c>
@@ -3770,7 +3776,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>42</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>42</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>42</v>
       </c>
@@ -3839,7 +3845,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>42</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>42</v>
       </c>
@@ -3885,7 +3891,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>42</v>
       </c>
@@ -3908,7 +3914,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>42</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>42</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>42</v>
       </c>
@@ -3977,7 +3983,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>42</v>
       </c>
@@ -4000,7 +4006,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>42</v>
       </c>
@@ -4023,7 +4029,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>42</v>
       </c>
@@ -4046,7 +4052,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -4069,7 +4075,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>42</v>
       </c>
@@ -4092,7 +4098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>42</v>
       </c>
@@ -4115,7 +4121,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>42</v>
       </c>
@@ -4138,7 +4144,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>42</v>
       </c>
@@ -4161,7 +4167,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>42</v>
       </c>
@@ -4184,7 +4190,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>42</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -4230,7 +4236,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>42</v>
       </c>
@@ -4253,7 +4259,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>42</v>
       </c>
@@ -4276,7 +4282,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>42</v>
       </c>
@@ -4299,7 +4305,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>42</v>
       </c>
@@ -4322,7 +4328,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>42</v>
       </c>
@@ -4345,7 +4351,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -4368,7 +4374,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>42</v>
       </c>
@@ -4391,7 +4397,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>42</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>42</v>
       </c>
@@ -4437,7 +4443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>42</v>
       </c>
@@ -4460,7 +4466,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -4506,7 +4512,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>42</v>
       </c>
@@ -4542,18 +4548,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431E17FB-41C8-40BE-942D-5C20ADEE04C5}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -4570,7 +4576,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -4587,7 +4593,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -4604,7 +4610,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -4621,7 +4627,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -4638,7 +4644,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Updating spreadsheet column header to match notebook access
</commit_message>
<xml_diff>
--- a/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
+++ b/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rizwansaeed/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\forks\sample-notebooks\examples\use-cases\abor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4AB24D-ADC6-E041-86AE-F4B2B74A401A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2EF741-EB05-4083-8544-04F8933FC9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart Of Accounts" sheetId="1" r:id="rId1"/>
@@ -227,9 +227,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
   </si>
 </sst>
 </file>
@@ -666,17 +666,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.68359375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -684,64 +684,64 @@
         <v>60</v>
       </c>
       <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
       <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -758,14 +758,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -773,13 +773,13 @@
         <v>60</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -787,38 +787,38 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -832,41 +832,41 @@
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.83984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
       <c r="H1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -886,10 +886,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -909,10 +909,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -932,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -955,10 +955,10 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -978,10 +978,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1001,10 +1001,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1024,10 +1024,10 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1047,10 +1047,10 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1070,10 +1070,10 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1093,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1116,10 +1116,10 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1139,10 +1139,10 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1162,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1185,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1208,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1231,10 +1231,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1254,10 +1254,10 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1277,10 +1277,10 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1300,10 +1300,10 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1323,10 +1323,10 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1346,10 +1346,10 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1369,10 +1369,10 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1392,10 +1392,10 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1415,10 +1415,10 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1438,10 +1438,10 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1461,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1484,10 +1484,10 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1507,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1530,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1553,10 +1553,10 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1576,10 +1576,10 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1599,10 +1599,10 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1622,13 +1622,13 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1648,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1671,10 +1671,10 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1694,10 +1694,10 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1717,10 +1717,10 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1740,10 +1740,10 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1763,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1786,10 +1786,10 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1809,10 +1809,10 @@
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1832,10 +1832,10 @@
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1855,10 +1855,10 @@
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1878,10 +1878,10 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1901,10 +1901,10 @@
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1924,10 +1924,10 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1947,10 +1947,10 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1970,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1993,10 +1993,10 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2016,10 +2016,10 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2039,10 +2039,10 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -2062,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2085,18 +2085,18 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55">
         <v>100100</v>
@@ -2111,15 +2111,15 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56">
         <v>109900</v>
@@ -2134,15 +2134,15 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C57">
         <v>110100</v>
@@ -2157,15 +2157,15 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C58">
         <v>112100</v>
@@ -2180,15 +2180,15 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>42</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59">
         <v>119000</v>
@@ -2203,15 +2203,15 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60">
         <v>120000</v>
@@ -2226,15 +2226,15 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>42</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61">
         <v>141000</v>
@@ -2249,15 +2249,15 @@
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C62">
         <v>142200</v>
@@ -2272,15 +2272,15 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>42</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63">
         <v>143000</v>
@@ -2295,15 +2295,15 @@
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>42</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>145000</v>
@@ -2318,15 +2318,15 @@
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>42</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65">
         <v>149000</v>
@@ -2341,15 +2341,15 @@
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>42</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C66">
         <v>160000</v>
@@ -2364,15 +2364,15 @@
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C67">
         <v>160900</v>
@@ -2387,15 +2387,15 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C68">
         <v>162000</v>
@@ -2410,15 +2410,15 @@
         <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>42</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C69">
         <v>164000</v>
@@ -2433,15 +2433,15 @@
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>42</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70">
         <v>164200</v>
@@ -2456,15 +2456,15 @@
         <v>1</v>
       </c>
       <c r="G70" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>42</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C71">
         <v>180700</v>
@@ -2479,15 +2479,15 @@
         <v>1</v>
       </c>
       <c r="G71" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C72">
         <v>200100</v>
@@ -2502,15 +2502,15 @@
         <v>1</v>
       </c>
       <c r="G72" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>42</v>
       </c>
       <c r="B73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C73">
         <v>209900</v>
@@ -2525,15 +2525,15 @@
         <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>42</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C74">
         <v>210100</v>
@@ -2548,15 +2548,15 @@
         <v>1</v>
       </c>
       <c r="G74" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>42</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75">
         <v>212100</v>
@@ -2571,15 +2571,15 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>42</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C76">
         <v>219000</v>
@@ -2594,15 +2594,15 @@
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>42</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C77">
         <v>241000</v>
@@ -2617,15 +2617,15 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C78">
         <v>242200</v>
@@ -2640,18 +2640,18 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C79">
         <v>243000</v>
@@ -2666,15 +2666,15 @@
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>42</v>
       </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C80">
         <v>249000</v>
@@ -2689,15 +2689,15 @@
         <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>42</v>
       </c>
       <c r="B81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C81">
         <v>260000</v>
@@ -2712,15 +2712,15 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C82">
         <v>260900</v>
@@ -2735,15 +2735,15 @@
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>42</v>
       </c>
       <c r="B83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C83">
         <v>262000</v>
@@ -2758,15 +2758,15 @@
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C84">
         <v>264000</v>
@@ -2781,15 +2781,15 @@
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C85">
         <v>264200</v>
@@ -2804,15 +2804,15 @@
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>42</v>
       </c>
       <c r="B86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C86">
         <v>270100</v>
@@ -2827,15 +2827,15 @@
         <v>1</v>
       </c>
       <c r="G86" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C87">
         <v>300000</v>
@@ -2850,15 +2850,15 @@
         <v>1</v>
       </c>
       <c r="G87" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C88">
         <v>302000</v>
@@ -2873,15 +2873,15 @@
         <v>1</v>
       </c>
       <c r="G88" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>42</v>
       </c>
       <c r="B89" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C89">
         <v>309000</v>
@@ -2896,15 +2896,15 @@
         <v>1</v>
       </c>
       <c r="G89" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>42</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C90">
         <v>320000</v>
@@ -2919,15 +2919,15 @@
         <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>42</v>
       </c>
       <c r="B91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C91">
         <v>322000</v>
@@ -2942,15 +2942,15 @@
         <v>1</v>
       </c>
       <c r="G91" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>42</v>
       </c>
       <c r="B92" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C92">
         <v>329000</v>
@@ -2965,15 +2965,15 @@
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>42</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C93">
         <v>610100</v>
@@ -2988,15 +2988,15 @@
         <v>1</v>
       </c>
       <c r="G93" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>42</v>
       </c>
       <c r="B94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C94">
         <v>612100</v>
@@ -3011,15 +3011,15 @@
         <v>1</v>
       </c>
       <c r="G94" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>42</v>
       </c>
       <c r="B95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C95">
         <v>619000</v>
@@ -3034,15 +3034,15 @@
         <v>1</v>
       </c>
       <c r="G95" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>42</v>
       </c>
       <c r="B96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C96">
         <v>641000</v>
@@ -3057,15 +3057,15 @@
         <v>1</v>
       </c>
       <c r="G96" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>42</v>
       </c>
       <c r="B97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C97">
         <v>642200</v>
@@ -3080,15 +3080,15 @@
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>42</v>
       </c>
       <c r="B98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C98">
         <v>643000</v>
@@ -3103,15 +3103,15 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>42</v>
       </c>
       <c r="B99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C99">
         <v>645000</v>
@@ -3126,15 +3126,15 @@
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>42</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C100">
         <v>649000</v>
@@ -3149,15 +3149,15 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>42</v>
       </c>
       <c r="B101" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C101">
         <v>670000</v>
@@ -3172,15 +3172,15 @@
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>42</v>
       </c>
       <c r="B102" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C102">
         <v>641001</v>
@@ -3195,15 +3195,15 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>42</v>
       </c>
       <c r="B103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C103">
         <v>642000</v>
@@ -3218,15 +3218,15 @@
         <v>1</v>
       </c>
       <c r="G103" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>42</v>
       </c>
       <c r="B104" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C104">
         <v>643001</v>
@@ -3241,15 +3241,15 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>42</v>
       </c>
       <c r="B105" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C105">
         <v>645001</v>
@@ -3264,15 +3264,15 @@
         <v>1</v>
       </c>
       <c r="G105" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>42</v>
       </c>
       <c r="B106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C106">
         <v>649001</v>
@@ -3287,15 +3287,15 @@
         <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C107">
         <v>770000</v>
@@ -3310,18 +3310,18 @@
         <v>1</v>
       </c>
       <c r="G107" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H107" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>42</v>
       </c>
       <c r="B108" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C108">
         <v>100100</v>
@@ -3336,15 +3336,15 @@
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>42</v>
       </c>
       <c r="B109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C109">
         <v>109900</v>
@@ -3359,15 +3359,15 @@
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>42</v>
       </c>
       <c r="B110" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C110">
         <v>110100</v>
@@ -3382,15 +3382,15 @@
         <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>42</v>
       </c>
       <c r="B111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C111">
         <v>112100</v>
@@ -3405,15 +3405,15 @@
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>42</v>
       </c>
       <c r="B112" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C112">
         <v>119000</v>
@@ -3428,15 +3428,15 @@
         <v>1</v>
       </c>
       <c r="G112" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>42</v>
       </c>
       <c r="B113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C113">
         <v>120000</v>
@@ -3451,15 +3451,15 @@
         <v>1</v>
       </c>
       <c r="G113" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>42</v>
       </c>
       <c r="B114" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C114">
         <v>141000</v>
@@ -3474,15 +3474,15 @@
         <v>1</v>
       </c>
       <c r="G114" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>42</v>
       </c>
       <c r="B115" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C115">
         <v>142200</v>
@@ -3497,15 +3497,15 @@
         <v>1</v>
       </c>
       <c r="G115" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>42</v>
       </c>
       <c r="B116" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C116">
         <v>143000</v>
@@ -3520,15 +3520,15 @@
         <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>42</v>
       </c>
       <c r="B117" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C117">
         <v>145000</v>
@@ -3543,15 +3543,15 @@
         <v>1</v>
       </c>
       <c r="G117" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>42</v>
       </c>
       <c r="B118" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C118">
         <v>149000</v>
@@ -3566,15 +3566,15 @@
         <v>1</v>
       </c>
       <c r="G118" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>42</v>
       </c>
       <c r="B119" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C119">
         <v>160000</v>
@@ -3589,15 +3589,15 @@
         <v>1</v>
       </c>
       <c r="G119" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>42</v>
       </c>
       <c r="B120" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C120">
         <v>160900</v>
@@ -3612,15 +3612,15 @@
         <v>1</v>
       </c>
       <c r="G120" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>42</v>
       </c>
       <c r="B121" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C121">
         <v>162000</v>
@@ -3635,15 +3635,15 @@
         <v>1</v>
       </c>
       <c r="G121" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>42</v>
       </c>
       <c r="B122" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C122">
         <v>164000</v>
@@ -3658,15 +3658,15 @@
         <v>1</v>
       </c>
       <c r="G122" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>42</v>
       </c>
       <c r="B123" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C123">
         <v>164200</v>
@@ -3681,15 +3681,15 @@
         <v>1</v>
       </c>
       <c r="G123" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>42</v>
       </c>
       <c r="B124" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C124">
         <v>180700</v>
@@ -3704,15 +3704,15 @@
         <v>1</v>
       </c>
       <c r="G124" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>42</v>
       </c>
       <c r="B125" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C125">
         <v>200100</v>
@@ -3727,15 +3727,15 @@
         <v>1</v>
       </c>
       <c r="G125" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>42</v>
       </c>
       <c r="B126" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C126">
         <v>209900</v>
@@ -3750,15 +3750,15 @@
         <v>1</v>
       </c>
       <c r="G126" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>42</v>
       </c>
       <c r="B127" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C127">
         <v>210100</v>
@@ -3773,15 +3773,15 @@
         <v>1</v>
       </c>
       <c r="G127" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>42</v>
       </c>
       <c r="B128" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C128">
         <v>212100</v>
@@ -3796,15 +3796,15 @@
         <v>1</v>
       </c>
       <c r="G128" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>42</v>
       </c>
       <c r="B129" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C129">
         <v>219000</v>
@@ -3819,15 +3819,15 @@
         <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>42</v>
       </c>
       <c r="B130" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C130">
         <v>241000</v>
@@ -3842,15 +3842,15 @@
         <v>1</v>
       </c>
       <c r="G130" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>42</v>
       </c>
       <c r="B131" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C131">
         <v>242200</v>
@@ -3865,15 +3865,15 @@
         <v>1</v>
       </c>
       <c r="G131" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>42</v>
       </c>
       <c r="B132" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C132">
         <v>243000</v>
@@ -3888,15 +3888,15 @@
         <v>1</v>
       </c>
       <c r="G132" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>42</v>
       </c>
       <c r="B133" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C133">
         <v>249000</v>
@@ -3911,15 +3911,15 @@
         <v>1</v>
       </c>
       <c r="G133" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>42</v>
       </c>
       <c r="B134" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C134">
         <v>260000</v>
@@ -3934,15 +3934,15 @@
         <v>1</v>
       </c>
       <c r="G134" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
         <v>42</v>
       </c>
       <c r="B135" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C135">
         <v>260900</v>
@@ -3957,15 +3957,15 @@
         <v>1</v>
       </c>
       <c r="G135" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>42</v>
       </c>
       <c r="B136" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C136">
         <v>262000</v>
@@ -3980,15 +3980,15 @@
         <v>1</v>
       </c>
       <c r="G136" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>42</v>
       </c>
       <c r="B137" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C137">
         <v>264000</v>
@@ -4003,15 +4003,15 @@
         <v>1</v>
       </c>
       <c r="G137" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
         <v>42</v>
       </c>
       <c r="B138" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C138">
         <v>264200</v>
@@ -4026,15 +4026,15 @@
         <v>1</v>
       </c>
       <c r="G138" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
         <v>42</v>
       </c>
       <c r="B139" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C139">
         <v>270100</v>
@@ -4049,15 +4049,15 @@
         <v>1</v>
       </c>
       <c r="G139" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>42</v>
       </c>
       <c r="B140" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C140">
         <v>300000</v>
@@ -4072,15 +4072,15 @@
         <v>1</v>
       </c>
       <c r="G140" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>42</v>
       </c>
       <c r="B141" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C141">
         <v>302000</v>
@@ -4095,15 +4095,15 @@
         <v>1</v>
       </c>
       <c r="G141" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
         <v>42</v>
       </c>
       <c r="B142" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C142">
         <v>309000</v>
@@ -4118,15 +4118,15 @@
         <v>1</v>
       </c>
       <c r="G142" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
         <v>42</v>
       </c>
       <c r="B143" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C143">
         <v>320000</v>
@@ -4141,15 +4141,15 @@
         <v>1</v>
       </c>
       <c r="G143" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
         <v>42</v>
       </c>
       <c r="B144" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C144">
         <v>322000</v>
@@ -4164,15 +4164,15 @@
         <v>1</v>
       </c>
       <c r="G144" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
         <v>42</v>
       </c>
       <c r="B145" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C145">
         <v>329000</v>
@@ -4187,15 +4187,15 @@
         <v>1</v>
       </c>
       <c r="G145" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
         <v>42</v>
       </c>
       <c r="B146" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C146">
         <v>610100</v>
@@ -4210,15 +4210,15 @@
         <v>1</v>
       </c>
       <c r="G146" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>42</v>
       </c>
       <c r="B147" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C147">
         <v>612100</v>
@@ -4233,15 +4233,15 @@
         <v>1</v>
       </c>
       <c r="G147" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
         <v>42</v>
       </c>
       <c r="B148" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C148">
         <v>619000</v>
@@ -4256,15 +4256,15 @@
         <v>1</v>
       </c>
       <c r="G148" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>42</v>
       </c>
       <c r="B149" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C149">
         <v>641000</v>
@@ -4279,15 +4279,15 @@
         <v>1</v>
       </c>
       <c r="G149" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>42</v>
       </c>
       <c r="B150" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C150">
         <v>642200</v>
@@ -4302,15 +4302,15 @@
         <v>1</v>
       </c>
       <c r="G150" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
         <v>42</v>
       </c>
       <c r="B151" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C151">
         <v>643000</v>
@@ -4325,15 +4325,15 @@
         <v>1</v>
       </c>
       <c r="G151" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
         <v>42</v>
       </c>
       <c r="B152" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C152">
         <v>645000</v>
@@ -4348,15 +4348,15 @@
         <v>1</v>
       </c>
       <c r="G152" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>42</v>
       </c>
       <c r="B153" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C153">
         <v>649000</v>
@@ -4371,15 +4371,15 @@
         <v>1</v>
       </c>
       <c r="G153" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
         <v>42</v>
       </c>
       <c r="B154" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C154">
         <v>670000</v>
@@ -4394,15 +4394,15 @@
         <v>1</v>
       </c>
       <c r="G154" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>42</v>
       </c>
       <c r="B155" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C155">
         <v>641001</v>
@@ -4417,15 +4417,15 @@
         <v>1</v>
       </c>
       <c r="G155" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
         <v>42</v>
       </c>
       <c r="B156" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C156">
         <v>642000</v>
@@ -4440,15 +4440,15 @@
         <v>1</v>
       </c>
       <c r="G156" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
         <v>42</v>
       </c>
       <c r="B157" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C157">
         <v>643001</v>
@@ -4463,15 +4463,15 @@
         <v>1</v>
       </c>
       <c r="G157" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>42</v>
       </c>
       <c r="B158" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C158">
         <v>645001</v>
@@ -4486,15 +4486,15 @@
         <v>1</v>
       </c>
       <c r="G158" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
         <v>42</v>
       </c>
       <c r="B159" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C159">
         <v>649001</v>
@@ -4509,15 +4509,15 @@
         <v>1</v>
       </c>
       <c r="G159" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
         <v>42</v>
       </c>
       <c r="B160" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C160">
         <v>770000</v>
@@ -4532,10 +4532,10 @@
         <v>1</v>
       </c>
       <c r="G160" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H160" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4552,31 +4552,31 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
       </c>
       <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -4587,13 +4587,13 @@
         <v>300000</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -4604,61 +4604,61 @@
         <v>770000</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>242200</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>770000</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <v>770000</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating spreadsheet column header to match notebook access (#733)
</commit_message>
<xml_diff>
--- a/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
+++ b/examples/use-cases/abor/data/chart-of-accounts-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rizwansaeed/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\forks\sample-notebooks\examples\use-cases\abor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4AB24D-ADC6-E041-86AE-F4B2B74A401A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2EF741-EB05-4083-8544-04F8933FC9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" xr2:uid="{A2DD0639-A52C-4ECD-8211-E545F32F9A41}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart Of Accounts" sheetId="1" r:id="rId1"/>
@@ -227,9 +227,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
   </si>
 </sst>
 </file>
@@ -666,17 +666,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.68359375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -684,64 +684,64 @@
         <v>60</v>
       </c>
       <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
       <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -758,14 +758,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -773,13 +773,13 @@
         <v>60</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -787,38 +787,38 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -832,41 +832,41 @@
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.83984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
       <c r="H1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -886,10 +886,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -909,10 +909,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -932,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -955,10 +955,10 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -978,10 +978,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1001,10 +1001,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1024,10 +1024,10 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1047,10 +1047,10 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1070,10 +1070,10 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1093,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1116,10 +1116,10 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1139,10 +1139,10 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1162,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1185,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1208,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1231,10 +1231,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1254,10 +1254,10 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1277,10 +1277,10 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1300,10 +1300,10 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1323,10 +1323,10 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1346,10 +1346,10 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1369,10 +1369,10 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1392,10 +1392,10 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1415,10 +1415,10 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1438,10 +1438,10 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1461,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1484,10 +1484,10 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1507,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1530,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1553,10 +1553,10 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1576,10 +1576,10 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1599,10 +1599,10 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1622,13 +1622,13 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1648,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1671,10 +1671,10 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1694,10 +1694,10 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1717,10 +1717,10 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1740,10 +1740,10 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1763,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1786,10 +1786,10 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1809,10 +1809,10 @@
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1832,10 +1832,10 @@
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1855,10 +1855,10 @@
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1878,10 +1878,10 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1901,10 +1901,10 @@
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1924,10 +1924,10 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1947,10 +1947,10 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1970,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1993,10 +1993,10 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2016,10 +2016,10 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2039,10 +2039,10 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -2062,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2085,18 +2085,18 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55">
         <v>100100</v>
@@ -2111,15 +2111,15 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56">
         <v>109900</v>
@@ -2134,15 +2134,15 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C57">
         <v>110100</v>
@@ -2157,15 +2157,15 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C58">
         <v>112100</v>
@@ -2180,15 +2180,15 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>42</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59">
         <v>119000</v>
@@ -2203,15 +2203,15 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60">
         <v>120000</v>
@@ -2226,15 +2226,15 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>42</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61">
         <v>141000</v>
@@ -2249,15 +2249,15 @@
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C62">
         <v>142200</v>
@@ -2272,15 +2272,15 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>42</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63">
         <v>143000</v>
@@ -2295,15 +2295,15 @@
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>42</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>145000</v>
@@ -2318,15 +2318,15 @@
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>42</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65">
         <v>149000</v>
@@ -2341,15 +2341,15 @@
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>42</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C66">
         <v>160000</v>
@@ -2364,15 +2364,15 @@
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C67">
         <v>160900</v>
@@ -2387,15 +2387,15 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C68">
         <v>162000</v>
@@ -2410,15 +2410,15 @@
         <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>42</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C69">
         <v>164000</v>
@@ -2433,15 +2433,15 @@
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>42</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70">
         <v>164200</v>
@@ -2456,15 +2456,15 @@
         <v>1</v>
       </c>
       <c r="G70" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>42</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C71">
         <v>180700</v>
@@ -2479,15 +2479,15 @@
         <v>1</v>
       </c>
       <c r="G71" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C72">
         <v>200100</v>
@@ -2502,15 +2502,15 @@
         <v>1</v>
       </c>
       <c r="G72" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>42</v>
       </c>
       <c r="B73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C73">
         <v>209900</v>
@@ -2525,15 +2525,15 @@
         <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>42</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C74">
         <v>210100</v>
@@ -2548,15 +2548,15 @@
         <v>1</v>
       </c>
       <c r="G74" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>42</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75">
         <v>212100</v>
@@ -2571,15 +2571,15 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>42</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C76">
         <v>219000</v>
@@ -2594,15 +2594,15 @@
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>42</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C77">
         <v>241000</v>
@@ -2617,15 +2617,15 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C78">
         <v>242200</v>
@@ -2640,18 +2640,18 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C79">
         <v>243000</v>
@@ -2666,15 +2666,15 @@
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>42</v>
       </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C80">
         <v>249000</v>
@@ -2689,15 +2689,15 @@
         <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>42</v>
       </c>
       <c r="B81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C81">
         <v>260000</v>
@@ -2712,15 +2712,15 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C82">
         <v>260900</v>
@@ -2735,15 +2735,15 @@
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>42</v>
       </c>
       <c r="B83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C83">
         <v>262000</v>
@@ -2758,15 +2758,15 @@
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C84">
         <v>264000</v>
@@ -2781,15 +2781,15 @@
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C85">
         <v>264200</v>
@@ -2804,15 +2804,15 @@
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>42</v>
       </c>
       <c r="B86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C86">
         <v>270100</v>
@@ -2827,15 +2827,15 @@
         <v>1</v>
       </c>
       <c r="G86" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C87">
         <v>300000</v>
@@ -2850,15 +2850,15 @@
         <v>1</v>
       </c>
       <c r="G87" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C88">
         <v>302000</v>
@@ -2873,15 +2873,15 @@
         <v>1</v>
       </c>
       <c r="G88" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>42</v>
       </c>
       <c r="B89" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C89">
         <v>309000</v>
@@ -2896,15 +2896,15 @@
         <v>1</v>
       </c>
       <c r="G89" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>42</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C90">
         <v>320000</v>
@@ -2919,15 +2919,15 @@
         <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>42</v>
       </c>
       <c r="B91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C91">
         <v>322000</v>
@@ -2942,15 +2942,15 @@
         <v>1</v>
       </c>
       <c r="G91" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>42</v>
       </c>
       <c r="B92" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C92">
         <v>329000</v>
@@ -2965,15 +2965,15 @@
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>42</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C93">
         <v>610100</v>
@@ -2988,15 +2988,15 @@
         <v>1</v>
       </c>
       <c r="G93" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>42</v>
       </c>
       <c r="B94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C94">
         <v>612100</v>
@@ -3011,15 +3011,15 @@
         <v>1</v>
       </c>
       <c r="G94" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>42</v>
       </c>
       <c r="B95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C95">
         <v>619000</v>
@@ -3034,15 +3034,15 @@
         <v>1</v>
       </c>
       <c r="G95" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>42</v>
       </c>
       <c r="B96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C96">
         <v>641000</v>
@@ -3057,15 +3057,15 @@
         <v>1</v>
       </c>
       <c r="G96" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>42</v>
       </c>
       <c r="B97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C97">
         <v>642200</v>
@@ -3080,15 +3080,15 @@
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>42</v>
       </c>
       <c r="B98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C98">
         <v>643000</v>
@@ -3103,15 +3103,15 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>42</v>
       </c>
       <c r="B99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C99">
         <v>645000</v>
@@ -3126,15 +3126,15 @@
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>42</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C100">
         <v>649000</v>
@@ -3149,15 +3149,15 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>42</v>
       </c>
       <c r="B101" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C101">
         <v>670000</v>
@@ -3172,15 +3172,15 @@
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>42</v>
       </c>
       <c r="B102" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C102">
         <v>641001</v>
@@ -3195,15 +3195,15 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>42</v>
       </c>
       <c r="B103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C103">
         <v>642000</v>
@@ -3218,15 +3218,15 @@
         <v>1</v>
       </c>
       <c r="G103" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>42</v>
       </c>
       <c r="B104" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C104">
         <v>643001</v>
@@ -3241,15 +3241,15 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>42</v>
       </c>
       <c r="B105" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C105">
         <v>645001</v>
@@ -3264,15 +3264,15 @@
         <v>1</v>
       </c>
       <c r="G105" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>42</v>
       </c>
       <c r="B106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C106">
         <v>649001</v>
@@ -3287,15 +3287,15 @@
         <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C107">
         <v>770000</v>
@@ -3310,18 +3310,18 @@
         <v>1</v>
       </c>
       <c r="G107" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H107" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>42</v>
       </c>
       <c r="B108" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C108">
         <v>100100</v>
@@ -3336,15 +3336,15 @@
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>42</v>
       </c>
       <c r="B109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C109">
         <v>109900</v>
@@ -3359,15 +3359,15 @@
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>42</v>
       </c>
       <c r="B110" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C110">
         <v>110100</v>
@@ -3382,15 +3382,15 @@
         <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>42</v>
       </c>
       <c r="B111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C111">
         <v>112100</v>
@@ -3405,15 +3405,15 @@
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>42</v>
       </c>
       <c r="B112" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C112">
         <v>119000</v>
@@ -3428,15 +3428,15 @@
         <v>1</v>
       </c>
       <c r="G112" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>42</v>
       </c>
       <c r="B113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C113">
         <v>120000</v>
@@ -3451,15 +3451,15 @@
         <v>1</v>
       </c>
       <c r="G113" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>42</v>
       </c>
       <c r="B114" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C114">
         <v>141000</v>
@@ -3474,15 +3474,15 @@
         <v>1</v>
       </c>
       <c r="G114" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>42</v>
       </c>
       <c r="B115" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C115">
         <v>142200</v>
@@ -3497,15 +3497,15 @@
         <v>1</v>
       </c>
       <c r="G115" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>42</v>
       </c>
       <c r="B116" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C116">
         <v>143000</v>
@@ -3520,15 +3520,15 @@
         <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>42</v>
       </c>
       <c r="B117" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C117">
         <v>145000</v>
@@ -3543,15 +3543,15 @@
         <v>1</v>
       </c>
       <c r="G117" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>42</v>
       </c>
       <c r="B118" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C118">
         <v>149000</v>
@@ -3566,15 +3566,15 @@
         <v>1</v>
       </c>
       <c r="G118" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>42</v>
       </c>
       <c r="B119" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C119">
         <v>160000</v>
@@ -3589,15 +3589,15 @@
         <v>1</v>
       </c>
       <c r="G119" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>42</v>
       </c>
       <c r="B120" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C120">
         <v>160900</v>
@@ -3612,15 +3612,15 @@
         <v>1</v>
       </c>
       <c r="G120" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>42</v>
       </c>
       <c r="B121" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C121">
         <v>162000</v>
@@ -3635,15 +3635,15 @@
         <v>1</v>
       </c>
       <c r="G121" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>42</v>
       </c>
       <c r="B122" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C122">
         <v>164000</v>
@@ -3658,15 +3658,15 @@
         <v>1</v>
       </c>
       <c r="G122" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>42</v>
       </c>
       <c r="B123" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C123">
         <v>164200</v>
@@ -3681,15 +3681,15 @@
         <v>1</v>
       </c>
       <c r="G123" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>42</v>
       </c>
       <c r="B124" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C124">
         <v>180700</v>
@@ -3704,15 +3704,15 @@
         <v>1</v>
       </c>
       <c r="G124" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>42</v>
       </c>
       <c r="B125" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C125">
         <v>200100</v>
@@ -3727,15 +3727,15 @@
         <v>1</v>
       </c>
       <c r="G125" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>42</v>
       </c>
       <c r="B126" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C126">
         <v>209900</v>
@@ -3750,15 +3750,15 @@
         <v>1</v>
       </c>
       <c r="G126" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>42</v>
       </c>
       <c r="B127" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C127">
         <v>210100</v>
@@ -3773,15 +3773,15 @@
         <v>1</v>
       </c>
       <c r="G127" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>42</v>
       </c>
       <c r="B128" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C128">
         <v>212100</v>
@@ -3796,15 +3796,15 @@
         <v>1</v>
       </c>
       <c r="G128" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>42</v>
       </c>
       <c r="B129" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C129">
         <v>219000</v>
@@ -3819,15 +3819,15 @@
         <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>42</v>
       </c>
       <c r="B130" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C130">
         <v>241000</v>
@@ -3842,15 +3842,15 @@
         <v>1</v>
       </c>
       <c r="G130" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>42</v>
       </c>
       <c r="B131" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C131">
         <v>242200</v>
@@ -3865,15 +3865,15 @@
         <v>1</v>
       </c>
       <c r="G131" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>42</v>
       </c>
       <c r="B132" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C132">
         <v>243000</v>
@@ -3888,15 +3888,15 @@
         <v>1</v>
       </c>
       <c r="G132" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>42</v>
       </c>
       <c r="B133" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C133">
         <v>249000</v>
@@ -3911,15 +3911,15 @@
         <v>1</v>
       </c>
       <c r="G133" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>42</v>
       </c>
       <c r="B134" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C134">
         <v>260000</v>
@@ -3934,15 +3934,15 @@
         <v>1</v>
       </c>
       <c r="G134" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
         <v>42</v>
       </c>
       <c r="B135" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C135">
         <v>260900</v>
@@ -3957,15 +3957,15 @@
         <v>1</v>
       </c>
       <c r="G135" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>42</v>
       </c>
       <c r="B136" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C136">
         <v>262000</v>
@@ -3980,15 +3980,15 @@
         <v>1</v>
       </c>
       <c r="G136" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>42</v>
       </c>
       <c r="B137" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C137">
         <v>264000</v>
@@ -4003,15 +4003,15 @@
         <v>1</v>
       </c>
       <c r="G137" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
         <v>42</v>
       </c>
       <c r="B138" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C138">
         <v>264200</v>
@@ -4026,15 +4026,15 @@
         <v>1</v>
       </c>
       <c r="G138" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
         <v>42</v>
       </c>
       <c r="B139" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C139">
         <v>270100</v>
@@ -4049,15 +4049,15 @@
         <v>1</v>
       </c>
       <c r="G139" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>42</v>
       </c>
       <c r="B140" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C140">
         <v>300000</v>
@@ -4072,15 +4072,15 @@
         <v>1</v>
       </c>
       <c r="G140" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>42</v>
       </c>
       <c r="B141" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C141">
         <v>302000</v>
@@ -4095,15 +4095,15 @@
         <v>1</v>
       </c>
       <c r="G141" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
         <v>42</v>
       </c>
       <c r="B142" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C142">
         <v>309000</v>
@@ -4118,15 +4118,15 @@
         <v>1</v>
       </c>
       <c r="G142" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
         <v>42</v>
       </c>
       <c r="B143" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C143">
         <v>320000</v>
@@ -4141,15 +4141,15 @@
         <v>1</v>
       </c>
       <c r="G143" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
         <v>42</v>
       </c>
       <c r="B144" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C144">
         <v>322000</v>
@@ -4164,15 +4164,15 @@
         <v>1</v>
       </c>
       <c r="G144" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
         <v>42</v>
       </c>
       <c r="B145" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C145">
         <v>329000</v>
@@ -4187,15 +4187,15 @@
         <v>1</v>
       </c>
       <c r="G145" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
         <v>42</v>
       </c>
       <c r="B146" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C146">
         <v>610100</v>
@@ -4210,15 +4210,15 @@
         <v>1</v>
       </c>
       <c r="G146" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>42</v>
       </c>
       <c r="B147" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C147">
         <v>612100</v>
@@ -4233,15 +4233,15 @@
         <v>1</v>
       </c>
       <c r="G147" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
         <v>42</v>
       </c>
       <c r="B148" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C148">
         <v>619000</v>
@@ -4256,15 +4256,15 @@
         <v>1</v>
       </c>
       <c r="G148" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>42</v>
       </c>
       <c r="B149" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C149">
         <v>641000</v>
@@ -4279,15 +4279,15 @@
         <v>1</v>
       </c>
       <c r="G149" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>42</v>
       </c>
       <c r="B150" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C150">
         <v>642200</v>
@@ -4302,15 +4302,15 @@
         <v>1</v>
       </c>
       <c r="G150" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
         <v>42</v>
       </c>
       <c r="B151" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C151">
         <v>643000</v>
@@ -4325,15 +4325,15 @@
         <v>1</v>
       </c>
       <c r="G151" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
         <v>42</v>
       </c>
       <c r="B152" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C152">
         <v>645000</v>
@@ -4348,15 +4348,15 @@
         <v>1</v>
       </c>
       <c r="G152" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>42</v>
       </c>
       <c r="B153" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C153">
         <v>649000</v>
@@ -4371,15 +4371,15 @@
         <v>1</v>
       </c>
       <c r="G153" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
         <v>42</v>
       </c>
       <c r="B154" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C154">
         <v>670000</v>
@@ -4394,15 +4394,15 @@
         <v>1</v>
       </c>
       <c r="G154" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>42</v>
       </c>
       <c r="B155" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C155">
         <v>641001</v>
@@ -4417,15 +4417,15 @@
         <v>1</v>
       </c>
       <c r="G155" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
         <v>42</v>
       </c>
       <c r="B156" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C156">
         <v>642000</v>
@@ -4440,15 +4440,15 @@
         <v>1</v>
       </c>
       <c r="G156" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
         <v>42</v>
       </c>
       <c r="B157" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C157">
         <v>643001</v>
@@ -4463,15 +4463,15 @@
         <v>1</v>
       </c>
       <c r="G157" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>42</v>
       </c>
       <c r="B158" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C158">
         <v>645001</v>
@@ -4486,15 +4486,15 @@
         <v>1</v>
       </c>
       <c r="G158" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
         <v>42</v>
       </c>
       <c r="B159" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C159">
         <v>649001</v>
@@ -4509,15 +4509,15 @@
         <v>1</v>
       </c>
       <c r="G159" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
         <v>42</v>
       </c>
       <c r="B160" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C160">
         <v>770000</v>
@@ -4532,10 +4532,10 @@
         <v>1</v>
       </c>
       <c r="G160" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H160" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4552,31 +4552,31 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
       </c>
       <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -4587,13 +4587,13 @@
         <v>300000</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -4604,61 +4604,61 @@
         <v>770000</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>242200</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>770000</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <v>770000</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>